<commit_message>
Criando Forms web rpa
</commit_message>
<xml_diff>
--- a/Projects RPA with excel/Project_Capture_Address_With_CNPJ/data_cnpj.xlsx
+++ b/Projects RPA with excel/Project_Capture_Address_With_CNPJ/data_cnpj.xlsx
@@ -15,17 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>CNPJ</t>
   </si>
   <si>
+    <t>14.380.200/0001-21</t>
+  </si>
+  <si>
+    <t>43.828.151/0001-45</t>
+  </si>
+  <si>
+    <t>29.979.036/0001-40</t>
+  </si>
+  <si>
     <t>60.316.817/0001-03</t>
   </si>
   <si>
-    <t>14380200000121</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
@@ -39,21 +45,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>IFOOD.COM AGENCIA DE RESTAURANTES ONLINE S.A.</t>
-  </si>
-  <si>
-    <t>ATIVA</t>
-  </si>
-  <si>
-    <t>Atividades de intermediação e agenciamento de serviços e negócios em geral, exceto imobiliários</t>
-  </si>
-  <si>
-    <t>06.020-902</t>
-  </si>
-  <si>
-    <t>juridico@ifood.com.br</t>
   </si>
 </sst>
 </file>
@@ -400,16 +391,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="62.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="21.862142857142857" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
@@ -419,39 +410,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -484,14 +455,18 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>